<commit_message>
added cost for sarah & dream square
</commit_message>
<xml_diff>
--- a/recreate/expense_tracking.xlsx
+++ b/recreate/expense_tracking.xlsx
@@ -1,24 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ulab_course_materials\recreate\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC656EDC-8AC1-4ED5-BF8E-BA8583A82856}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="21840" windowHeight="13740" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="brac_cdm" sheetId="1" r:id="rId1"/>
     <sheet name="dream_square" sheetId="2" r:id="rId2"/>
+    <sheet name="sarah" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -32,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="34">
   <si>
     <t>Name</t>
   </si>
@@ -139,8 +134,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -168,8 +163,34 @@
       <name val="Garamond"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Garamond"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -185,6 +206,17 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -213,12 +245,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -226,11 +260,21 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
     <cellStyle name="20% - Accent6" xfId="2" builtinId="50"/>
+    <cellStyle name="40% - Accent2" xfId="4" builtinId="35"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Warning Text" xfId="3" builtinId="11"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -288,7 +332,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -323,7 +367,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -500,43 +544,41 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="30.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" style="1"/>
-    <col min="4" max="4" width="20.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" style="1"/>
+    <col min="4" max="4" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" style="1"/>
-    <col min="9" max="9" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" style="1"/>
+    <col min="9" max="9" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.88671875" style="1"/>
-    <col min="14" max="14" width="17.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.85546875" style="1"/>
+    <col min="14" max="14" width="17.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="8.88671875" style="1"/>
+    <col min="16" max="16" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" s="2" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -577,7 +619,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -623,7 +665,7 @@
         <v>188750</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -665,7 +707,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -707,7 +749,7 @@
         <v>37750</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -729,7 +771,7 @@
         <v>56000</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -737,7 +779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -745,7 +787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -753,7 +795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
@@ -761,7 +803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
@@ -769,7 +811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
@@ -777,7 +819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17">
       <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
@@ -785,7 +827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17">
       <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
@@ -793,7 +835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17">
       <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
@@ -801,7 +843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17">
       <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
@@ -809,7 +851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17">
       <c r="A16" s="3">
         <f>ROWS(A2:A15)</f>
         <v>14</v>
@@ -819,7 +861,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2">
       <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
@@ -827,7 +869,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2">
       <c r="A18" s="3" t="s">
         <v>16</v>
       </c>
@@ -835,7 +877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2">
       <c r="A19" s="3">
         <f>ROWS(A17:A18)</f>
         <v>2</v>
@@ -852,36 +894,36 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92D3D871-4B12-4DA8-896C-3506F9CBE073}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="30.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" style="1"/>
-    <col min="4" max="4" width="20.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" style="1"/>
-    <col min="9" max="9" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.88671875" style="1"/>
-    <col min="14" max="14" width="17.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="31.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" style="1"/>
+    <col min="4" max="4" width="21.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" style="1"/>
+    <col min="9" max="9" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.85546875" style="1"/>
+    <col min="14" max="14" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" s="2" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -900,6 +942,351 @@
       <c r="G1" s="6" t="s">
         <v>24</v>
       </c>
+      <c r="I1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="O1" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q1" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="11">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="12">
+        <v>7000</v>
+      </c>
+      <c r="F2" s="12">
+        <f>B16</f>
+        <v>7</v>
+      </c>
+      <c r="G2" s="12">
+        <f>E2*F2</f>
+        <v>49000</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="11">
+        <v>0</v>
+      </c>
+      <c r="K2" s="11">
+        <f>A$16+A$19</f>
+        <v>16</v>
+      </c>
+      <c r="L2" s="11">
+        <f>J2*K2</f>
+        <v>0</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="O2" s="13">
+        <v>0.15</v>
+      </c>
+      <c r="Q2" s="14">
+        <f>G5+L5+O4</f>
+        <v>156500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="11">
+        <v>0</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="12">
+        <v>5500</v>
+      </c>
+      <c r="F3" s="12">
+        <f>B19</f>
+        <v>2</v>
+      </c>
+      <c r="G3" s="12">
+        <f t="shared" ref="G3:G4" si="0">E3*F3</f>
+        <v>11000</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" s="11">
+        <v>1100</v>
+      </c>
+      <c r="K3" s="11">
+        <f t="shared" ref="K3:K4" si="1">A$16+A$19</f>
+        <v>16</v>
+      </c>
+      <c r="L3" s="11">
+        <f t="shared" ref="L3:L4" si="2">J3*K3</f>
+        <v>17600</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="O3" s="13">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="11">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="12">
+        <v>30000</v>
+      </c>
+      <c r="F4" s="12">
+        <v>1</v>
+      </c>
+      <c r="G4" s="12">
+        <f t="shared" si="0"/>
+        <v>30000</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" s="11">
+        <v>1100</v>
+      </c>
+      <c r="K4" s="11">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="L4" s="11">
+        <f t="shared" si="2"/>
+        <v>17600</v>
+      </c>
+      <c r="N4" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="O4" s="13">
+        <f>(G5+L5)*(O2+O3)</f>
+        <v>31300</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="11">
+        <v>0</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="12">
+        <f>SUM(G2:G4)</f>
+        <v>90000</v>
+      </c>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="11">
+        <f>SUM(L2:L4)</f>
+        <v>35200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="A7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="A8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="A9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="A10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="A11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="A12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="A13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="A14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
+      <c r="A15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17">
+      <c r="A16" s="11">
+        <f>ROWS(A2:A15)</f>
+        <v>14</v>
+      </c>
+      <c r="B16" s="11">
+        <f>SUM(B2:B15)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="11">
+        <f>ROWS(A17:A18)</f>
+        <v>2</v>
+      </c>
+      <c r="B19" s="11">
+        <f>SUM(B17:B18)</f>
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:Q19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J3" sqref="J3:J4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="31.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" style="1"/>
+    <col min="4" max="4" width="21.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" style="1"/>
+    <col min="9" max="9" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.85546875" style="1"/>
+    <col min="14" max="14" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="8.85546875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" s="2" customFormat="1">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="I1" s="6" t="s">
         <v>25</v>
       </c>
@@ -922,7 +1309,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -932,8 +1319,8 @@
       <c r="D2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="5">
-        <v>9000</v>
+      <c r="E2" s="7">
+        <v>10500</v>
       </c>
       <c r="F2" s="5">
         <f>B16</f>
@@ -941,7 +1328,7 @@
       </c>
       <c r="G2" s="5">
         <f>E2*F2</f>
-        <v>63000</v>
+        <v>73500</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>26</v>
@@ -965,10 +1352,10 @@
       </c>
       <c r="Q2" s="5">
         <f>G5+L5+O4</f>
-        <v>188750</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+        <v>197125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -978,8 +1365,8 @@
       <c r="D3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="5">
-        <v>8000</v>
+      <c r="E3" s="7">
+        <v>10500</v>
       </c>
       <c r="F3" s="5">
         <f>B19</f>
@@ -987,13 +1374,13 @@
       </c>
       <c r="G3" s="5">
         <f t="shared" ref="G3:G4" si="0">E3*F3</f>
-        <v>16000</v>
+        <v>21000</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>27</v>
       </c>
       <c r="J3" s="5">
-        <v>1500</v>
+        <v>1400</v>
       </c>
       <c r="K3" s="5">
         <f t="shared" ref="K3:K4" si="1">A$16+A$19</f>
@@ -1001,7 +1388,7 @@
       </c>
       <c r="L3" s="5">
         <f t="shared" ref="L3:L4" si="2">J3*K3</f>
-        <v>24000</v>
+        <v>22400</v>
       </c>
       <c r="N3" s="5" t="s">
         <v>31</v>
@@ -1010,7 +1397,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -1034,7 +1421,7 @@
         <v>28</v>
       </c>
       <c r="J4" s="5">
-        <v>2000</v>
+        <v>1550</v>
       </c>
       <c r="K4" s="5">
         <f t="shared" si="1"/>
@@ -1042,17 +1429,17 @@
       </c>
       <c r="L4" s="5">
         <f t="shared" si="2"/>
-        <v>32000</v>
+        <v>24800</v>
       </c>
       <c r="N4" s="5" t="s">
         <v>32</v>
       </c>
       <c r="O4" s="5">
         <f>(G5+L5)*(O2+O3)</f>
-        <v>37750</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+        <v>39425</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -1064,17 +1451,17 @@
       <c r="F5" s="5"/>
       <c r="G5" s="5">
         <f>SUM(G2:G4)</f>
-        <v>95000</v>
+        <v>110500</v>
       </c>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
       <c r="L5" s="5">
         <f>SUM(L2:L4)</f>
-        <v>56000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+        <v>47200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -1082,7 +1469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -1090,7 +1477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -1098,7 +1485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
@@ -1106,7 +1493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
@@ -1114,7 +1501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
@@ -1122,7 +1509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17">
       <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
@@ -1130,7 +1517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17">
       <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
@@ -1138,7 +1525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17">
       <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
@@ -1146,7 +1533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17">
       <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
@@ -1154,7 +1541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17">
       <c r="A16" s="3">
         <f>ROWS(A2:A15)</f>
         <v>14</v>
@@ -1164,7 +1551,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2">
       <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
@@ -1172,7 +1559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2">
       <c r="A18" s="3" t="s">
         <v>16</v>
       </c>
@@ -1180,7 +1567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2">
       <c r="A19" s="3">
         <f>ROWS(A17:A18)</f>
         <v>2</v>

</xml_diff>